<commit_message>
Index and table upload 15.10
</commit_message>
<xml_diff>
--- a/texts_fin.xlsx
+++ b/texts_fin.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0000shakesp\0000Shakespeare-phrases-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0000shakesp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5226129-9C47-49E3-8358-4E6C6C3570B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C09E5B0-10AE-4102-B1AA-E39F5CFA976E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{BBE6E32D-62B2-4B13-BAAA-307AEDD5E135}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2160" uniqueCount="1330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2441" uniqueCount="1474">
   <si>
     <t>To be, or not to be,</t>
   </si>
@@ -4015,6 +4015,438 @@
   </si>
   <si>
     <t>wiltu niwiht weiter wesan?</t>
+  </si>
+  <si>
+    <t>ofr</t>
+  </si>
+  <si>
+    <t>301</t>
+  </si>
+  <si>
+    <t>'S is fei ned ols Gold, wos glensd.</t>
+  </si>
+  <si>
+    <t>Nothing will come of nothing.</t>
+  </si>
+  <si>
+    <t>Vo nix werrd nix.</t>
+  </si>
+  <si>
+    <t>Und nix kemmd vo nix.</t>
+  </si>
+  <si>
+    <t>All the world's a stage, and all the men and women merely players.</t>
+  </si>
+  <si>
+    <t>They have their exits and their entrances.</t>
+  </si>
+  <si>
+    <t>As You Like lt, Act 2, scene 7</t>
+  </si>
+  <si>
+    <t>Die Weld is a Deoda,</t>
+  </si>
+  <si>
+    <t>olle Menna und Weiba bloß Schauspiela,</t>
+  </si>
+  <si>
+    <t>die naus und nei genga.</t>
+  </si>
+  <si>
+    <t>There are more things in heaven and earth, Horatio,</t>
+  </si>
+  <si>
+    <t>S gibd einfach mehr uf f dea Weld,</t>
+  </si>
+  <si>
+    <t>als du denggsd. Dengg nur an Bimberleswichdi.</t>
+  </si>
+  <si>
+    <t>'S is nix gud oda schlechd, 's kummd drauf o,</t>
+  </si>
+  <si>
+    <t>wiesd drieba denggsd.</t>
+  </si>
+  <si>
+    <t>There's many a man has more hair than wit.</t>
+  </si>
+  <si>
+    <t>So vill hamm</t>
+  </si>
+  <si>
+    <t>mea Hoa uf fm Bulmos als Gribs drinna.</t>
+  </si>
+  <si>
+    <t>Lifes a tale told by an idiot, full of sound and fury, signifying nothing.</t>
+  </si>
+  <si>
+    <t>Des Lern is a Märla, voll Bimberleswichdi, wo a Depp derzähld.</t>
+  </si>
+  <si>
+    <t>Merry Wives of Windsor. Act 2, scene 2</t>
+  </si>
+  <si>
+    <t>Lieba zu fria als wie zu späd</t>
+  </si>
+  <si>
+    <t>Celerity is never more admired</t>
+  </si>
+  <si>
+    <t>Die Schnelln werrn vo kaan mera bewunnad</t>
+  </si>
+  <si>
+    <t>als wie vo die Schlofhaum.</t>
+  </si>
+  <si>
+    <t>and our little life is rounded with a sleep.</t>
+  </si>
+  <si>
+    <t>The Tempest, Act 4, scene 1 ·</t>
+  </si>
+  <si>
+    <t>Mir senn gmachd wie a Draam,</t>
+  </si>
+  <si>
+    <t>Wemmas ned zeichd, liebd ma a ned.</t>
+  </si>
+  <si>
+    <t>Doubt truth to be a liar, but never doubt 1love.</t>
+  </si>
+  <si>
+    <t>Glaab nix und gornix, bloß,</t>
+  </si>
+  <si>
+    <t>dass ich dich hobm mechd.</t>
+  </si>
+  <si>
+    <t>Twelf th Night, Act 3, scene 1</t>
+  </si>
+  <si>
+    <t>Sung is gud in da Lieb, gfunna werrn is bessa.</t>
+  </si>
+  <si>
+    <t>For which of my bad parts didst thou first</t>
+  </si>
+  <si>
+    <t>In welche meina Maggn hasdn dich zuersd vergnalld?</t>
+  </si>
+  <si>
+    <t>Twelf th Night, Act 1, scene l</t>
+  </si>
+  <si>
+    <t>Wenn die Mussigg die Lieb fuddard,</t>
+  </si>
+  <si>
+    <t>ess weida.</t>
+  </si>
+  <si>
+    <t>the more I give to thee, the more 1have,</t>
+  </si>
+  <si>
+    <t>Romeo and Juliet, Act 2, scene</t>
+  </si>
+  <si>
+    <t>Mei Lieb is so arch, je mehr ich da gib, desdo gressa werrds.</t>
+  </si>
+  <si>
+    <t>For I ne'er saw true beauty till this night.</t>
+  </si>
+  <si>
+    <t>Noch nie hob ich</t>
+  </si>
+  <si>
+    <t>so wos Scheens gseng wie heid Nachd.</t>
+  </si>
+  <si>
+    <t>Auf da Spua bleim woa bei da Lieb</t>
+  </si>
+  <si>
+    <t>scho immer schwer. Es ruggld scho mol.</t>
+  </si>
+  <si>
+    <t>I am one</t>
+  </si>
+  <si>
+    <t>who loved not wisely but too well.</t>
+  </si>
+  <si>
+    <t>Ich wor hold blind vor lauda Lieb.</t>
+  </si>
+  <si>
+    <t>=- Aha ned so brov.</t>
+  </si>
+  <si>
+    <t>As You Like lt, Act 2, scene 6</t>
+  </si>
+  <si>
+    <t>Liebe haud am des Vöchala naus.</t>
+  </si>
+  <si>
+    <t>but bears it out even to the edge of doom.</t>
+  </si>
+  <si>
+    <t>Liebe werrd ned älder bis zum End oller Doch.</t>
+  </si>
+  <si>
+    <t>A Mo spild im Lern</t>
+  </si>
+  <si>
+    <t>an hauf n Rolln. Und a Fraa aa.</t>
+  </si>
+  <si>
+    <t>Uneasy lies the head that wears the crown.</t>
+  </si>
+  <si>
+    <t>Mid aner Krona uffm Bulmos</t>
+  </si>
+  <si>
+    <t>ko ma schlechd schlofn.</t>
+  </si>
+  <si>
+    <t>Better a witty fool than a foolish wit.</t>
+  </si>
+  <si>
+    <t>Twelf th Night, Act 1, scene 5</t>
+  </si>
+  <si>
+    <t>Bessa a witziga Depp als a deppischa Witz.</t>
+  </si>
+  <si>
+    <t>Gerechd is schlechd</t>
+  </si>
+  <si>
+    <t>und schlechd is gerechd</t>
+  </si>
+  <si>
+    <t>A fool thinks himself to be w1•se,</t>
+  </si>
+  <si>
+    <t>but a wise man knows himself to be a fool.</t>
+  </si>
+  <si>
+    <t>As You Like lt, Act 5, scene 1</t>
+  </si>
+  <si>
+    <t>A Bleeda denggd, er is schlau,</t>
+  </si>
+  <si>
+    <t>aha a Schlaua was, dass er bleed is.</t>
+  </si>
+  <si>
+    <t>That one may smile, and smile,</t>
+  </si>
+  <si>
+    <t>Bees sa und lächeln gehd olles zwa</t>
+  </si>
+  <si>
+    <t>Love all, trust a few, do wrong to none.</t>
+  </si>
+  <si>
+    <t>Du sollsd die Leid meng, kamm draua</t>
+  </si>
+  <si>
+    <t>und a kamm wos Beses do.</t>
+  </si>
+  <si>
+    <t>Ich grabbl jedm inna Oasch,</t>
+  </si>
+  <si>
+    <t>dwer mir neigrabbld.</t>
+  </si>
+  <si>
+    <t>God hath given you one face, and you</t>
+  </si>
+  <si>
+    <t>Des Gsichd,</t>
+  </si>
+  <si>
+    <t>desd vom lieben God grichd hosd,</t>
+  </si>
+  <si>
+    <t>kennsd aa so lossn.</t>
+  </si>
+  <si>
+    <t>Neither a borrower nor a lender be:</t>
+  </si>
+  <si>
+    <t>for loan oft loses both itself and friend • • •</t>
+  </si>
+  <si>
+    <t>Du nix borgn und a nix leia, weil beim Verborgn verliasd ofd dein Kumpl</t>
+  </si>
+  <si>
+    <t>und beim Borng a wengla des Gfiel fias Geld.</t>
+  </si>
+  <si>
+    <t>Self-love, my liege, is not so vile a sin, as self-neglecting.</t>
+  </si>
+  <si>
+    <t>Wenn ich mich selba mooch, is des fei ned</t>
+  </si>
+  <si>
+    <t>so a greisliche Sünd wie, wenn ich mich ned mechad.</t>
+  </si>
+  <si>
+    <t>Machs so gud,</t>
+  </si>
+  <si>
+    <t>wiesd des gedachd hosd.</t>
+  </si>
+  <si>
+    <t>If we are true to ourselves, we can not be false</t>
+  </si>
+  <si>
+    <t>Wemma zu uns selba steh, kemma kan olieng.</t>
+  </si>
+  <si>
+    <t>And oftentimes excusing of a fault doth make the fault the worse.</t>
+  </si>
+  <si>
+    <t>Blos ned endschuldichn,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dodamid werrds noch schlimma.</t>
+  </si>
+  <si>
+    <t>1 wasted time,</t>
+  </si>
+  <si>
+    <t>and now doth time waste me.</t>
+  </si>
+  <si>
+    <t>Richard II, Act 5 , scene 5</t>
+  </si>
+  <si>
+    <t>Ich hob Zeid versandld, und etsa versandld die Zeid miech.</t>
+  </si>
+  <si>
+    <t>it is not enough to speak, but to speak true.</t>
+  </si>
+  <si>
+    <t>Des mergsd da: Waaf n reichd ned,</t>
+  </si>
+  <si>
+    <t>musd scho ehrlich sa. Und Wohrheid sogn.</t>
+  </si>
+  <si>
+    <t>Ich mechad,</t>
+  </si>
+  <si>
+    <t>dass mei Pfea so schnell rennd</t>
+  </si>
+  <si>
+    <t>wie dei Zunga.</t>
+  </si>
+  <si>
+    <t>I am not bound to please thee with my answer.</t>
+  </si>
+  <si>
+    <t>The Merchant of Venice, Act 4, scene 1</t>
+  </si>
+  <si>
+    <t>Dir brauchd mei Andword ned zu gfolln.</t>
+  </si>
+  <si>
+    <t>or eise my heart concealing it will break.</t>
+  </si>
+  <si>
+    <t>The Taming of the Shrew, Act 6, scene 3</t>
+  </si>
+  <si>
+    <t>Endweda sog ichs</t>
+  </si>
+  <si>
+    <t>oder mir zerfedzds die Brusd.</t>
+  </si>
+  <si>
+    <t>The grief that does not speak</t>
+  </si>
+  <si>
+    <t>knits up o-er wrought heart and bids it break.</t>
+  </si>
+  <si>
+    <t>Macbeth, Act 4, scene 3</t>
+  </si>
+  <si>
+    <t>Spuggs aus,</t>
+  </si>
+  <si>
+    <t>sonsd zerreißds dich.</t>
+  </si>
+  <si>
+    <t>Give every man thine ear, but few thy voice.</t>
+  </si>
+  <si>
+    <t>Horch jedm zu,</t>
+  </si>
+  <si>
+    <t>aba loss dia ned vo jedm wos sogn.</t>
+  </si>
+  <si>
+    <t>When I think, Imust speak.</t>
+  </si>
+  <si>
+    <t>Bei mir lichd des Geherrn auf der Zunga.</t>
+  </si>
+  <si>
+    <t>Werrder flieng</t>
+  </si>
+  <si>
+    <t>Hamlet, Act3, scene 3</t>
+  </si>
+  <si>
+    <t>they are seldome spent in vaine. Richard II., Act 2, scene 1</t>
+  </si>
+  <si>
+    <t>Da Deifl</t>
+  </si>
+  <si>
+    <t>schlachd aa die Bibl</t>
+  </si>
+  <si>
+    <t>fia sich aus.</t>
+  </si>
+  <si>
+    <t>King Lear, Act 3, scene 2</t>
+  </si>
+  <si>
+    <t>Vill Wizla</t>
+  </si>
+  <si>
+    <t>hom an wohrn Kern.</t>
+  </si>
+  <si>
+    <t>It is a kind of good deed to say well;</t>
+  </si>
+  <si>
+    <t>S is gud, wos Guds zu sogn</t>
+  </si>
+  <si>
+    <t>aba musd a wos Guds do.</t>
+  </si>
+  <si>
+    <t>Gschissn und gredd</t>
+  </si>
+  <si>
+    <t>is schnell a Haufn.</t>
+  </si>
+  <si>
+    <t>Ma sterbd bloß a mol.</t>
+  </si>
+  <si>
+    <t>Loss mich so, wie ich bin,</t>
+  </si>
+  <si>
+    <t>und nergl ned an mia rum.</t>
+  </si>
+  <si>
+    <t>Soll ich so weidamachn?</t>
+  </si>
+  <si>
+    <t>Oda ned?</t>
+  </si>
+  <si>
+    <t>Des is die Froch.</t>
   </si>
 </sst>
 </file>
@@ -4057,12 +4489,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4379,16 +4814,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A074AB5-1EF9-487A-9681-DA97360C2616}">
-  <dimension ref="A1:Q291"/>
+  <dimension ref="A1:Q344"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A291"/>
+      <selection activeCell="A342" sqref="A1:A344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" style="2"/>
-    <col min="2" max="3" width="11.5546875" style="1"/>
+    <col min="2" max="2" width="11.5546875" style="1"/>
+    <col min="3" max="3" width="11.5546875" style="2"/>
     <col min="4" max="4" width="37.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.88671875" style="1" customWidth="1"/>
@@ -4409,7 +4845,7 @@
       <c r="B1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="2">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -4438,7 +4874,7 @@
       <c r="B2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -4470,7 +4906,7 @@
       <c r="B3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -4496,7 +4932,7 @@
       <c r="B4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -4537,7 +4973,7 @@
       <c r="B5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -4572,7 +5008,7 @@
       <c r="B6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -4601,7 +5037,7 @@
       <c r="B7" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -4636,7 +5072,7 @@
       <c r="B8" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -4671,7 +5107,7 @@
       <c r="B9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -4706,7 +5142,7 @@
       <c r="B10" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -4735,7 +5171,7 @@
       <c r="B11" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -4776,7 +5212,7 @@
       <c r="B12" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -4802,7 +5238,7 @@
       <c r="B13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -4834,7 +5270,7 @@
       <c r="B14" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <v>14</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -4863,7 +5299,7 @@
       <c r="B15" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>15</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -4901,7 +5337,7 @@
       <c r="B16" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -4930,7 +5366,7 @@
       <c r="B17" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -4959,7 +5395,7 @@
       <c r="B18" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <v>18</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -4985,7 +5421,7 @@
       <c r="B19" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="2">
         <v>19</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -5008,7 +5444,7 @@
       <c r="B20" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="2">
         <v>20</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -5037,7 +5473,7 @@
       <c r="B21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="2">
         <v>21</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -5063,7 +5499,7 @@
       <c r="B22" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="2">
         <v>22</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -5098,7 +5534,7 @@
       <c r="B23" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="2">
         <v>23</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -5124,7 +5560,7 @@
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="2">
         <v>24</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -5150,7 +5586,7 @@
       <c r="B25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="2">
         <v>25</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -5182,7 +5618,7 @@
       <c r="B26" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="2">
         <v>26</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -5220,7 +5656,7 @@
       <c r="B27" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="2">
         <v>27</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -5252,7 +5688,7 @@
       <c r="B28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="2">
         <v>28</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -5281,7 +5717,7 @@
       <c r="B29" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="2">
         <v>29</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -5307,7 +5743,7 @@
       <c r="B30" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="2">
         <v>30</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -5339,7 +5775,7 @@
       <c r="B31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="2">
         <v>31</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -5368,7 +5804,7 @@
       <c r="B32" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="2">
         <v>32</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -5403,7 +5839,7 @@
       <c r="B33" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="2">
         <v>33</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -5432,7 +5868,7 @@
       <c r="B34" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="2">
         <v>34</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -5467,7 +5903,7 @@
       <c r="B35" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="2">
         <v>35</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -5508,7 +5944,7 @@
       <c r="B36" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="2">
         <v>36</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -5543,7 +5979,7 @@
       <c r="B37" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="2">
         <v>37</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -5575,7 +6011,7 @@
       <c r="B38" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="2">
         <v>38</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -5601,7 +6037,7 @@
       <c r="B39" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="2">
         <v>39</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -5639,7 +6075,7 @@
       <c r="B40" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="2">
         <v>40</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -5674,7 +6110,7 @@
       <c r="B41" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="2">
         <v>41</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -5703,7 +6139,7 @@
       <c r="B42" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="2">
         <v>42</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -5732,7 +6168,7 @@
       <c r="B43" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="2">
         <v>43</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -5758,7 +6194,7 @@
       <c r="B44" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="2">
         <v>44</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -5787,7 +6223,7 @@
       <c r="B45" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="2">
         <v>45</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -5819,7 +6255,7 @@
       <c r="B46" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="2">
         <v>46</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -5848,7 +6284,7 @@
       <c r="B47" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="2">
         <v>47</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -5877,7 +6313,7 @@
       <c r="B48" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="2">
         <v>201</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -5906,7 +6342,7 @@
       <c r="B49" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49" s="2">
         <v>202</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -5935,7 +6371,7 @@
       <c r="B50" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="2">
         <v>203</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -5958,7 +6394,7 @@
       <c r="B51" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="2">
         <v>204</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -5987,7 +6423,7 @@
       <c r="B52" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="2">
         <v>205</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -6016,7 +6452,7 @@
       <c r="B53" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="2">
         <v>206</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -6042,7 +6478,7 @@
       <c r="B54" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="2">
         <v>207</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -6077,7 +6513,7 @@
       <c r="B55" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="2">
         <v>208</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -6109,7 +6545,7 @@
       <c r="B56" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="2">
         <v>209</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -6141,7 +6577,7 @@
       <c r="B57" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57" s="2">
         <v>210</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -6164,7 +6600,7 @@
       <c r="B58" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58" s="2">
         <v>211</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -6190,7 +6626,7 @@
       <c r="B59" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="2">
         <v>212</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -6222,7 +6658,7 @@
       <c r="B60" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60" s="2">
         <v>213</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -6248,7 +6684,7 @@
       <c r="B61" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="2">
         <v>214</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -6280,7 +6716,7 @@
       <c r="B62" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="2">
         <v>215</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -6318,7 +6754,7 @@
       <c r="B63" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63" s="2">
         <v>216</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -6344,7 +6780,7 @@
       <c r="B64" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="2">
         <v>217</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -6364,7 +6800,7 @@
       <c r="B65" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="2">
         <v>218</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -6390,7 +6826,7 @@
       <c r="B66" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="2">
         <v>219</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -6413,7 +6849,7 @@
       <c r="B67" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="2">
         <v>220</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -6439,7 +6875,7 @@
       <c r="B68" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C68" s="2">
         <v>221</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -6468,7 +6904,7 @@
       <c r="B69" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="2">
         <v>222</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -6497,7 +6933,7 @@
       <c r="B70" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C70" s="2">
         <v>223</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -6520,7 +6956,7 @@
       <c r="B71" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C71" s="1">
+      <c r="C71" s="2">
         <v>224</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -6546,7 +6982,7 @@
       <c r="B72" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C72" s="2">
         <v>225</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -6572,7 +7008,7 @@
       <c r="B73" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C73" s="2">
         <v>226</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -6607,7 +7043,7 @@
       <c r="B74" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C74" s="1">
+      <c r="C74" s="2">
         <v>227</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -6630,7 +7066,7 @@
       <c r="B75" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="2">
         <v>228</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -6659,7 +7095,7 @@
       <c r="B76" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="2">
         <v>229</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -6682,7 +7118,7 @@
       <c r="B77" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="2">
         <v>230</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -6708,7 +7144,7 @@
       <c r="B78" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="2">
         <v>231</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -6731,7 +7167,7 @@
       <c r="B79" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C79" s="2">
         <v>232</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -6757,7 +7193,7 @@
       <c r="B80" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C80" s="2">
         <v>233</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -6783,7 +7219,7 @@
       <c r="B81" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="2">
         <v>234</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -6812,7 +7248,7 @@
       <c r="B82" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="2">
         <v>235</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -6841,7 +7277,7 @@
       <c r="B83" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C83" s="1">
+      <c r="C83" s="2">
         <v>236</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -6876,7 +7312,7 @@
       <c r="B84" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C84" s="1">
+      <c r="C84" s="2">
         <v>237</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -6908,7 +7344,7 @@
       <c r="B85" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C85" s="1">
+      <c r="C85" s="2">
         <v>238</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -6934,7 +7370,7 @@
       <c r="B86" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C86" s="2">
         <v>239</v>
       </c>
       <c r="D86" s="1" t="s">
@@ -6966,7 +7402,7 @@
       <c r="B87" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="2">
         <v>240</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -6992,7 +7428,7 @@
       <c r="B88" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C88" s="2">
         <v>241</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -7021,7 +7457,7 @@
       <c r="B89" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C89" s="1">
+      <c r="C89" s="2">
         <v>242</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -7047,7 +7483,7 @@
       <c r="B90" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C90" s="1">
+      <c r="C90" s="2">
         <v>243</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -7073,7 +7509,7 @@
       <c r="B91" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C91" s="1">
+      <c r="C91" s="2">
         <v>244</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -7099,7 +7535,7 @@
       <c r="B92" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C92" s="1">
+      <c r="C92" s="2">
         <v>245</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -7128,7 +7564,7 @@
       <c r="B93" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C93" s="1">
+      <c r="C93" s="2">
         <v>246</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -7154,7 +7590,7 @@
       <c r="B94" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="2">
         <v>247</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -7177,7 +7613,7 @@
       <c r="B95" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C95" s="1">
+      <c r="C95" s="2">
         <v>248</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -7209,7 +7645,7 @@
       <c r="B96" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C96" s="1">
+      <c r="C96" s="2">
         <v>701</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -7235,7 +7671,7 @@
       <c r="B97" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="2">
         <v>702</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -7258,7 +7694,7 @@
       <c r="B98" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="2">
         <v>703</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -7284,7 +7720,7 @@
       <c r="B99" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C99" s="1">
+      <c r="C99" s="2">
         <v>704</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -7319,7 +7755,7 @@
       <c r="B100" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C100" s="1">
+      <c r="C100" s="2">
         <v>705</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -7351,7 +7787,7 @@
       <c r="B101" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="2">
         <v>706</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -7377,7 +7813,7 @@
       <c r="B102" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C102" s="1">
+      <c r="C102" s="2">
         <v>707</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -7406,7 +7842,7 @@
       <c r="B103" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C103" s="1">
+      <c r="C103" s="2">
         <v>708</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -7438,7 +7874,7 @@
       <c r="B104" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C104" s="1">
+      <c r="C104" s="2">
         <v>709</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -7464,7 +7900,7 @@
       <c r="B105" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="2">
         <v>710</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -7490,7 +7926,7 @@
       <c r="B106" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C106" s="1">
+      <c r="C106" s="2">
         <v>711</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -7522,7 +7958,7 @@
       <c r="B107" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C107" s="1">
+      <c r="C107" s="2">
         <v>712</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -7551,7 +7987,7 @@
       <c r="B108" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C108" s="1">
+      <c r="C108" s="2">
         <v>713</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -7583,7 +8019,7 @@
       <c r="B109" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C109" s="1">
+      <c r="C109" s="2">
         <v>714</v>
       </c>
       <c r="D109" s="1" t="s">
@@ -7612,7 +8048,7 @@
       <c r="B110" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C110" s="1">
+      <c r="C110" s="2">
         <v>715</v>
       </c>
       <c r="D110" s="1" t="s">
@@ -7641,7 +8077,7 @@
       <c r="B111" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="2">
         <v>716</v>
       </c>
       <c r="D111" s="1" t="s">
@@ -7676,7 +8112,7 @@
       <c r="B112" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="2">
         <v>717</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -7705,7 +8141,7 @@
       <c r="B113" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C113" s="1">
+      <c r="C113" s="2">
         <v>718</v>
       </c>
       <c r="D113" s="1" t="s">
@@ -7737,7 +8173,7 @@
       <c r="B114" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C114" s="1">
+      <c r="C114" s="2">
         <v>719</v>
       </c>
       <c r="D114" s="1" t="s">
@@ -7769,7 +8205,7 @@
       <c r="B115" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C115" s="1">
+      <c r="C115" s="2">
         <v>720</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -7795,7 +8231,7 @@
       <c r="B116" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C116" s="1">
+      <c r="C116" s="2">
         <v>721</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -7821,7 +8257,7 @@
       <c r="B117" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="2">
         <v>722</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -7853,7 +8289,7 @@
       <c r="B118" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="2">
         <v>723</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -7879,7 +8315,7 @@
       <c r="B119" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="2">
         <v>724</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -7905,7 +8341,7 @@
       <c r="B120" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="2">
         <v>725</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -7931,7 +8367,7 @@
       <c r="B121" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="2">
         <v>726</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -7960,7 +8396,7 @@
       <c r="B122" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C122" s="1">
+      <c r="C122" s="2">
         <v>727</v>
       </c>
       <c r="D122" s="1" t="s">
@@ -7998,7 +8434,7 @@
       <c r="B123" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C123" s="1">
+      <c r="C123" s="2">
         <v>728</v>
       </c>
       <c r="D123" s="1" t="s">
@@ -8024,7 +8460,7 @@
       <c r="B124" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C124" s="1">
+      <c r="C124" s="2">
         <v>729</v>
       </c>
       <c r="D124" s="1" t="s">
@@ -8053,7 +8489,7 @@
       <c r="B125" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="2">
         <v>730</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -8079,7 +8515,7 @@
       <c r="B126" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="2">
         <v>731</v>
       </c>
       <c r="D126" s="1" t="s">
@@ -8114,7 +8550,7 @@
       <c r="B127" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="2">
         <v>732</v>
       </c>
       <c r="D127" s="1" t="s">
@@ -8143,7 +8579,7 @@
       <c r="B128" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="2">
         <v>733</v>
       </c>
       <c r="D128" s="1" t="s">
@@ -8172,7 +8608,7 @@
       <c r="B129" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="2">
         <v>734</v>
       </c>
       <c r="D129" s="1" t="s">
@@ -8201,7 +8637,7 @@
       <c r="B130" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="2">
         <v>735</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -8230,7 +8666,7 @@
       <c r="B131" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="2">
         <v>736</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -8259,7 +8695,7 @@
       <c r="B132" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="2">
         <v>737</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -8291,7 +8727,7 @@
       <c r="B133" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="2">
         <v>738</v>
       </c>
       <c r="D133" s="1" t="s">
@@ -8320,7 +8756,7 @@
       <c r="B134" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="2">
         <v>739</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -8346,7 +8782,7 @@
       <c r="B135" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="2">
         <v>740</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -8381,7 +8817,7 @@
       <c r="B136" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="2">
         <v>741</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -8407,7 +8843,7 @@
       <c r="B137" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C137" s="1">
+      <c r="C137" s="2">
         <v>742</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -8430,7 +8866,7 @@
       <c r="B138" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C138" s="1">
+      <c r="C138" s="2">
         <v>743</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -8459,7 +8895,7 @@
       <c r="B139" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C139" s="1">
+      <c r="C139" s="2">
         <v>744</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -8488,7 +8924,7 @@
       <c r="B140" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="2">
         <v>745</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -8517,7 +8953,7 @@
       <c r="B141" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="2">
         <v>746</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -8543,7 +8979,7 @@
       <c r="B142" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="2">
         <v>747</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -8569,7 +9005,7 @@
       <c r="B143" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C143" s="1">
+      <c r="C143" s="2">
         <v>748</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -8595,7 +9031,7 @@
       <c r="B144" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="2">
         <v>749</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -8615,7 +9051,7 @@
       <c r="B145" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="2">
         <v>750</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -8638,7 +9074,7 @@
       <c r="B146" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="2">
         <v>401</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -8667,7 +9103,7 @@
       <c r="B147" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="2">
         <v>402</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -8693,7 +9129,7 @@
       <c r="B148" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="2">
         <v>403</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -8725,7 +9161,7 @@
       <c r="B149" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C149" s="1">
+      <c r="C149" s="2">
         <v>404</v>
       </c>
       <c r="D149" s="1" t="s">
@@ -8763,7 +9199,7 @@
       <c r="B150" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="2">
         <v>405</v>
       </c>
       <c r="D150" s="1" t="s">
@@ -8801,7 +9237,7 @@
       <c r="B151" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="2">
         <v>406</v>
       </c>
       <c r="D151" s="1" t="s">
@@ -8830,7 +9266,7 @@
       <c r="B152" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="2">
         <v>407</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -8865,7 +9301,7 @@
       <c r="B153" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="2">
         <v>408</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -8897,7 +9333,7 @@
       <c r="B154" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="2">
         <v>409</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -8938,7 +9374,7 @@
       <c r="B155" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="2">
         <v>410</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -8967,7 +9403,7 @@
       <c r="B156" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C156" s="1">
+      <c r="C156" s="2">
         <v>411</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -8996,7 +9432,7 @@
       <c r="B157" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="2">
         <v>412</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -9028,7 +9464,7 @@
       <c r="B158" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="2">
         <v>413</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -9066,7 +9502,7 @@
       <c r="B159" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C159" s="1">
+      <c r="C159" s="2">
         <v>414</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -9104,7 +9540,7 @@
       <c r="B160" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C160" s="1">
+      <c r="C160" s="2">
         <v>415</v>
       </c>
       <c r="D160" s="1" t="s">
@@ -9130,7 +9566,7 @@
       <c r="B161" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C161" s="1">
+      <c r="C161" s="2">
         <v>416</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -9162,7 +9598,7 @@
       <c r="B162" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="2">
         <v>417</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -9185,7 +9621,7 @@
       <c r="B163" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="2">
         <v>418</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -9217,7 +9653,7 @@
       <c r="B164" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C164" s="1">
+      <c r="C164" s="2">
         <v>419</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -9246,7 +9682,7 @@
       <c r="B165" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C165" s="1">
+      <c r="C165" s="2">
         <v>420</v>
       </c>
       <c r="D165" s="1" t="s">
@@ -9278,7 +9714,7 @@
       <c r="B166" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C166" s="1">
+      <c r="C166" s="2">
         <v>421</v>
       </c>
       <c r="D166" s="1" t="s">
@@ -9307,7 +9743,7 @@
       <c r="B167" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C167" s="1">
+      <c r="C167" s="2">
         <v>422</v>
       </c>
       <c r="D167" s="1" t="s">
@@ -9339,7 +9775,7 @@
       <c r="B168" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C168" s="1">
+      <c r="C168" s="2">
         <v>423</v>
       </c>
       <c r="D168" s="1" t="s">
@@ -9365,7 +9801,7 @@
       <c r="B169" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C169" s="1">
+      <c r="C169" s="2">
         <v>424</v>
       </c>
       <c r="D169" s="1" t="s">
@@ -9391,7 +9827,7 @@
       <c r="B170" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C170" s="1">
+      <c r="C170" s="2">
         <v>425</v>
       </c>
       <c r="D170" s="1" t="s">
@@ -9429,7 +9865,7 @@
       <c r="B171" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C171" s="1">
+      <c r="C171" s="2">
         <v>426</v>
       </c>
       <c r="D171" s="1" t="s">
@@ -9458,7 +9894,7 @@
       <c r="B172" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C172" s="1">
+      <c r="C172" s="2">
         <v>427</v>
       </c>
       <c r="D172" s="1" t="s">
@@ -9487,7 +9923,7 @@
       <c r="B173" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C173" s="1">
+      <c r="C173" s="2">
         <v>428</v>
       </c>
       <c r="D173" s="1" t="s">
@@ -9516,7 +9952,7 @@
       <c r="B174" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C174" s="1">
+      <c r="C174" s="2">
         <v>429</v>
       </c>
       <c r="D174" s="1" t="s">
@@ -9542,7 +9978,7 @@
       <c r="B175" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C175" s="1">
+      <c r="C175" s="2">
         <v>430</v>
       </c>
       <c r="D175" s="1" t="s">
@@ -9577,7 +10013,7 @@
       <c r="B176" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C176" s="1">
+      <c r="C176" s="2">
         <v>431</v>
       </c>
       <c r="D176" s="1" t="s">
@@ -9609,7 +10045,7 @@
       <c r="B177" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C177" s="1">
+      <c r="C177" s="2">
         <v>432</v>
       </c>
       <c r="D177" s="1" t="s">
@@ -9641,7 +10077,7 @@
       <c r="B178" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C178" s="1">
+      <c r="C178" s="2">
         <v>433</v>
       </c>
       <c r="D178" s="1" t="s">
@@ -9667,7 +10103,7 @@
       <c r="B179" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C179" s="1">
+      <c r="C179" s="2">
         <v>434</v>
       </c>
       <c r="D179" s="1" t="s">
@@ -9705,7 +10141,7 @@
       <c r="B180" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C180" s="1">
+      <c r="C180" s="2">
         <v>435</v>
       </c>
       <c r="D180" s="1" t="s">
@@ -9743,7 +10179,7 @@
       <c r="B181" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C181" s="1">
+      <c r="C181" s="2">
         <v>436</v>
       </c>
       <c r="D181" s="1" t="s">
@@ -9775,7 +10211,7 @@
       <c r="B182" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C182" s="1">
+      <c r="C182" s="2">
         <v>437</v>
       </c>
       <c r="D182" s="1" t="s">
@@ -9810,7 +10246,7 @@
       <c r="B183" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C183" s="1">
+      <c r="C183" s="2">
         <v>438</v>
       </c>
       <c r="D183" s="1" t="s">
@@ -9836,7 +10272,7 @@
       <c r="B184" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C184" s="1">
+      <c r="C184" s="2">
         <v>439</v>
       </c>
       <c r="D184" s="1" t="s">
@@ -9874,7 +10310,7 @@
       <c r="B185" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C185" s="1">
+      <c r="C185" s="2">
         <v>440</v>
       </c>
       <c r="D185" s="1" t="s">
@@ -9903,7 +10339,7 @@
       <c r="B186" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C186" s="1">
+      <c r="C186" s="2">
         <v>441</v>
       </c>
       <c r="D186" s="1" t="s">
@@ -9932,7 +10368,7 @@
       <c r="B187" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C187" s="1">
+      <c r="C187" s="2">
         <v>442</v>
       </c>
       <c r="D187" s="1" t="s">
@@ -9961,7 +10397,7 @@
       <c r="B188" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C188" s="1">
+      <c r="C188" s="2">
         <v>443</v>
       </c>
       <c r="D188" s="1" t="s">
@@ -9993,7 +10429,7 @@
       <c r="B189" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C189" s="1">
+      <c r="C189" s="2">
         <v>444</v>
       </c>
       <c r="D189" s="1" t="s">
@@ -10022,7 +10458,7 @@
       <c r="B190" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C190" s="1">
+      <c r="C190" s="2">
         <v>445</v>
       </c>
       <c r="D190" s="1" t="s">
@@ -10048,7 +10484,7 @@
       <c r="B191" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C191" s="1">
+      <c r="C191" s="2">
         <v>446</v>
       </c>
       <c r="D191" s="1" t="s">
@@ -10074,7 +10510,7 @@
       <c r="B192" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C192" s="1">
+      <c r="C192" s="2">
         <v>447</v>
       </c>
       <c r="D192" s="1" t="s">
@@ -10106,7 +10542,7 @@
       <c r="B193" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C193" s="1">
+      <c r="C193" s="2">
         <v>101</v>
       </c>
       <c r="D193" s="1" t="s">
@@ -10138,7 +10574,7 @@
       <c r="B194" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C194" s="1">
+      <c r="C194" s="2">
         <v>102</v>
       </c>
       <c r="D194" s="1" t="s">
@@ -10173,7 +10609,7 @@
       <c r="B195" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C195" s="1">
+      <c r="C195" s="2">
         <v>103</v>
       </c>
       <c r="D195" s="1" t="s">
@@ -10199,7 +10635,7 @@
       <c r="B196" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C196" s="1">
+      <c r="C196" s="2">
         <v>104</v>
       </c>
       <c r="D196" s="1" t="s">
@@ -10240,7 +10676,7 @@
       <c r="B197" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C197" s="1">
+      <c r="C197" s="2">
         <v>105</v>
       </c>
       <c r="D197" s="1" t="s">
@@ -10284,7 +10720,7 @@
       <c r="B198" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C198" s="1">
+      <c r="C198" s="2">
         <v>106</v>
       </c>
       <c r="D198" s="1" t="s">
@@ -10313,7 +10749,7 @@
       <c r="B199" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C199" s="1">
+      <c r="C199" s="2">
         <v>107</v>
       </c>
       <c r="D199" s="1" t="s">
@@ -10351,7 +10787,7 @@
       <c r="B200" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C200" s="1">
+      <c r="C200" s="2">
         <v>108</v>
       </c>
       <c r="D200" s="1" t="s">
@@ -10392,7 +10828,7 @@
       <c r="B201" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C201" s="1">
+      <c r="C201" s="2">
         <v>109</v>
       </c>
       <c r="D201" s="1" t="s">
@@ -10430,7 +10866,7 @@
       <c r="B202" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C202" s="1">
+      <c r="C202" s="2">
         <v>110</v>
       </c>
       <c r="D202" s="1" t="s">
@@ -10480,7 +10916,7 @@
       <c r="B203" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C203" s="1">
+      <c r="C203" s="2">
         <v>111</v>
       </c>
       <c r="D203" s="1" t="s">
@@ -10515,7 +10951,7 @@
       <c r="B204" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C204" s="1">
+      <c r="C204" s="2">
         <v>112</v>
       </c>
       <c r="D204" s="1" t="s">
@@ -10541,7 +10977,7 @@
       <c r="B205" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C205" s="1">
+      <c r="C205" s="2">
         <v>113</v>
       </c>
       <c r="D205" s="1" t="s">
@@ -10591,7 +11027,7 @@
       <c r="B206" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C206" s="1">
+      <c r="C206" s="2">
         <v>114</v>
       </c>
       <c r="D206" s="1" t="s">
@@ -10623,7 +11059,7 @@
       <c r="B207" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C207" s="1">
+      <c r="C207" s="2">
         <v>115</v>
       </c>
       <c r="D207" s="1" t="s">
@@ -10655,7 +11091,7 @@
       <c r="B208" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C208" s="1">
+      <c r="C208" s="2">
         <v>116</v>
       </c>
       <c r="D208" s="1" t="s">
@@ -10684,7 +11120,7 @@
       <c r="B209" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C209" s="1">
+      <c r="C209" s="2">
         <v>117</v>
       </c>
       <c r="D209" s="1" t="s">
@@ -10728,7 +11164,7 @@
       <c r="B210" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C210" s="1">
+      <c r="C210" s="2">
         <v>118</v>
       </c>
       <c r="D210" s="1" t="s">
@@ -10757,7 +11193,7 @@
       <c r="B211" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C211" s="1">
+      <c r="C211" s="2">
         <v>119</v>
       </c>
       <c r="D211" s="1" t="s">
@@ -10786,7 +11222,7 @@
       <c r="B212" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C212" s="1">
+      <c r="C212" s="2">
         <v>120</v>
       </c>
       <c r="D212" s="1" t="s">
@@ -10815,7 +11251,7 @@
       <c r="B213" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C213" s="1">
+      <c r="C213" s="2">
         <v>121</v>
       </c>
       <c r="D213" s="1" t="s">
@@ -10844,7 +11280,7 @@
       <c r="B214" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C214" s="1">
+      <c r="C214" s="2">
         <v>122</v>
       </c>
       <c r="D214" s="1" t="s">
@@ -10873,7 +11309,7 @@
       <c r="B215" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C215" s="1">
+      <c r="C215" s="2">
         <v>123</v>
       </c>
       <c r="D215" s="1" t="s">
@@ -10902,7 +11338,7 @@
       <c r="B216" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C216" s="1">
+      <c r="C216" s="2">
         <v>124</v>
       </c>
       <c r="D216" s="1" t="s">
@@ -10931,7 +11367,7 @@
       <c r="B217" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C217" s="1">
+      <c r="C217" s="2">
         <v>125</v>
       </c>
       <c r="D217" s="1" t="s">
@@ -10957,7 +11393,7 @@
       <c r="B218" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C218" s="1">
+      <c r="C218" s="2">
         <v>126</v>
       </c>
       <c r="D218" s="1" t="s">
@@ -11001,7 +11437,7 @@
       <c r="B219" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C219" s="1">
+      <c r="C219" s="2">
         <v>127</v>
       </c>
       <c r="D219" s="1" t="s">
@@ -11033,7 +11469,7 @@
       <c r="B220" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C220" s="1">
+      <c r="C220" s="2">
         <v>128</v>
       </c>
       <c r="D220" s="1" t="s">
@@ -11065,7 +11501,7 @@
       <c r="B221" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C221" s="1">
+      <c r="C221" s="2">
         <v>129</v>
       </c>
       <c r="D221" s="1" t="s">
@@ -11091,7 +11527,7 @@
       <c r="B222" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C222" s="1">
+      <c r="C222" s="2">
         <v>130</v>
       </c>
       <c r="D222" s="1" t="s">
@@ -11129,7 +11565,7 @@
       <c r="B223" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C223" s="1">
+      <c r="C223" s="2">
         <v>131</v>
       </c>
       <c r="D223" s="1" t="s">
@@ -11158,7 +11594,7 @@
       <c r="B224" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C224" s="1">
+      <c r="C224" s="2">
         <v>132</v>
       </c>
       <c r="D224" s="1" t="s">
@@ -11193,7 +11629,7 @@
       <c r="B225" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C225" s="1">
+      <c r="C225" s="2">
         <v>133</v>
       </c>
       <c r="D225" s="1" t="s">
@@ -11231,7 +11667,7 @@
       <c r="B226" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C226" s="1">
+      <c r="C226" s="2">
         <v>134</v>
       </c>
       <c r="D226" s="1" t="s">
@@ -11266,7 +11702,7 @@
       <c r="B227" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C227" s="1">
+      <c r="C227" s="2">
         <v>135</v>
       </c>
       <c r="D227" s="1" t="s">
@@ -11301,7 +11737,7 @@
       <c r="B228" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C228" s="1">
+      <c r="C228" s="2">
         <v>136</v>
       </c>
       <c r="D228" s="1" t="s">
@@ -11327,7 +11763,7 @@
       <c r="B229" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C229" s="1">
+      <c r="C229" s="2">
         <v>137</v>
       </c>
       <c r="D229" s="1" t="s">
@@ -11365,7 +11801,7 @@
       <c r="B230" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C230" s="1">
+      <c r="C230" s="2">
         <v>138</v>
       </c>
       <c r="D230" s="1" t="s">
@@ -11391,7 +11827,7 @@
       <c r="B231" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C231" s="1">
+      <c r="C231" s="2">
         <v>139</v>
       </c>
       <c r="D231" s="1" t="s">
@@ -11426,7 +11862,7 @@
       <c r="B232" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C232" s="1">
+      <c r="C232" s="2">
         <v>140</v>
       </c>
       <c r="D232" s="1" t="s">
@@ -11464,7 +11900,7 @@
       <c r="B233" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C233" s="1">
+      <c r="C233" s="2">
         <v>141</v>
       </c>
       <c r="D233" s="1" t="s">
@@ -11499,7 +11935,7 @@
       <c r="B234" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C234" s="1">
+      <c r="C234" s="2">
         <v>142</v>
       </c>
       <c r="D234" s="1" t="s">
@@ -11531,7 +11967,7 @@
       <c r="B235" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C235" s="1">
+      <c r="C235" s="2">
         <v>143</v>
       </c>
       <c r="D235" s="1" t="s">
@@ -11563,7 +11999,7 @@
       <c r="B236" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C236" s="1">
+      <c r="C236" s="2">
         <v>144</v>
       </c>
       <c r="D236" s="1" t="s">
@@ -11595,7 +12031,7 @@
       <c r="B237" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C237" s="1">
+      <c r="C237" s="2">
         <v>145</v>
       </c>
       <c r="D237" s="1" t="s">
@@ -11615,7 +12051,7 @@
       <c r="B238" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C238" s="1">
+      <c r="C238" s="2">
         <v>146</v>
       </c>
       <c r="D238" s="1" t="s">
@@ -11638,7 +12074,7 @@
       <c r="B239" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C239" s="1">
+      <c r="C239" s="2">
         <v>147</v>
       </c>
       <c r="D239" s="1" t="s">
@@ -11676,7 +12112,7 @@
       <c r="B240" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C240" s="1">
+      <c r="C240" s="2">
         <v>148</v>
       </c>
       <c r="D240" s="1" t="s">
@@ -11702,7 +12138,7 @@
       <c r="B241" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C241" s="1">
+      <c r="C241" s="2">
         <v>149</v>
       </c>
       <c r="D241" s="1" t="s">
@@ -11728,7 +12164,7 @@
       <c r="B242" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="C242" s="1">
+      <c r="C242" s="2">
         <v>150</v>
       </c>
       <c r="D242" s="1" t="s">
@@ -11760,7 +12196,7 @@
       <c r="B243" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C243" s="1">
+      <c r="C243" s="2">
         <v>501</v>
       </c>
       <c r="D243" s="1" t="s">
@@ -11792,7 +12228,7 @@
       <c r="B244" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C244" s="1">
+      <c r="C244" s="2">
         <v>502</v>
       </c>
       <c r="D244" s="1" t="s">
@@ -11824,7 +12260,7 @@
       <c r="B245" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C245" s="1">
+      <c r="C245" s="2">
         <v>503</v>
       </c>
       <c r="D245" s="1" t="s">
@@ -11856,7 +12292,7 @@
       <c r="B246" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C246" s="1">
+      <c r="C246" s="2">
         <v>504</v>
       </c>
       <c r="D246" s="1" t="s">
@@ -11888,7 +12324,7 @@
       <c r="B247" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C247" s="1">
+      <c r="C247" s="2">
         <v>505</v>
       </c>
       <c r="D247" s="1" t="s">
@@ -11917,7 +12353,7 @@
       <c r="B248" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C248" s="1">
+      <c r="C248" s="2">
         <v>506</v>
       </c>
       <c r="D248" s="1" t="s">
@@ -11940,7 +12376,7 @@
       <c r="B249" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C249" s="1">
+      <c r="C249" s="2">
         <v>507</v>
       </c>
       <c r="D249" s="1" t="s">
@@ -11966,7 +12402,7 @@
       <c r="B250" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C250" s="1">
+      <c r="C250" s="2">
         <v>508</v>
       </c>
       <c r="D250" s="1" t="s">
@@ -12001,7 +12437,7 @@
       <c r="B251" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C251" s="1">
+      <c r="C251" s="2">
         <v>509</v>
       </c>
       <c r="D251" s="1" t="s">
@@ -12033,7 +12469,7 @@
       <c r="B252" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C252" s="1">
+      <c r="C252" s="2">
         <v>510</v>
       </c>
       <c r="D252" s="1" t="s">
@@ -12062,7 +12498,7 @@
       <c r="B253" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C253" s="1">
+      <c r="C253" s="2">
         <v>511</v>
       </c>
       <c r="D253" s="1" t="s">
@@ -12088,7 +12524,7 @@
       <c r="B254" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C254" s="1">
+      <c r="C254" s="2">
         <v>512</v>
       </c>
       <c r="D254" s="1" t="s">
@@ -12120,7 +12556,7 @@
       <c r="B255" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C255" s="1">
+      <c r="C255" s="2">
         <v>513</v>
       </c>
       <c r="D255" s="1" t="s">
@@ -12155,7 +12591,7 @@
       <c r="B256" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C256" s="1">
+      <c r="C256" s="2">
         <v>514</v>
       </c>
       <c r="D256" s="1" t="s">
@@ -12178,7 +12614,7 @@
       <c r="B257" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C257" s="1">
+      <c r="C257" s="2">
         <v>515</v>
       </c>
       <c r="D257" s="1" t="s">
@@ -12204,7 +12640,7 @@
       <c r="B258" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C258" s="1">
+      <c r="C258" s="2">
         <v>516</v>
       </c>
       <c r="D258" s="1" t="s">
@@ -12239,7 +12675,7 @@
       <c r="B259" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C259" s="1">
+      <c r="C259" s="2">
         <v>517</v>
       </c>
       <c r="D259" s="1" t="s">
@@ -12271,7 +12707,7 @@
       <c r="B260" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C260" s="1">
+      <c r="C260" s="2">
         <v>518</v>
       </c>
       <c r="D260" s="1" t="s">
@@ -12303,7 +12739,7 @@
       <c r="B261" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C261" s="1">
+      <c r="C261" s="2">
         <v>519</v>
       </c>
       <c r="D261" s="1" t="s">
@@ -12323,7 +12759,7 @@
       <c r="B262" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C262" s="1">
+      <c r="C262" s="2">
         <v>520</v>
       </c>
       <c r="D262" s="1" t="s">
@@ -12346,7 +12782,7 @@
       <c r="B263" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C263" s="1">
+      <c r="C263" s="2">
         <v>521</v>
       </c>
       <c r="D263" s="1" t="s">
@@ -12375,7 +12811,7 @@
       <c r="B264" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C264" s="1">
+      <c r="C264" s="2">
         <v>522</v>
       </c>
       <c r="D264" s="1" t="s">
@@ -12404,7 +12840,7 @@
       <c r="B265" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C265" s="1">
+      <c r="C265" s="2">
         <v>523</v>
       </c>
       <c r="D265" s="1" t="s">
@@ -12430,7 +12866,7 @@
       <c r="B266" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C266" s="1">
+      <c r="C266" s="2">
         <v>524</v>
       </c>
       <c r="D266" s="1" t="s">
@@ -12468,7 +12904,7 @@
       <c r="B267" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C267" s="1">
+      <c r="C267" s="2">
         <v>525</v>
       </c>
       <c r="D267" s="1" t="s">
@@ -12494,7 +12930,7 @@
       <c r="B268" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C268" s="1">
+      <c r="C268" s="2">
         <v>526</v>
       </c>
       <c r="D268" s="1" t="s">
@@ -12526,7 +12962,7 @@
       <c r="B269" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C269" s="1">
+      <c r="C269" s="2">
         <v>527</v>
       </c>
       <c r="D269" s="1" t="s">
@@ -12552,7 +12988,7 @@
       <c r="B270" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C270" s="1">
+      <c r="C270" s="2">
         <v>528</v>
       </c>
       <c r="D270" s="1" t="s">
@@ -12581,7 +13017,7 @@
       <c r="B271" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C271" s="1">
+      <c r="C271" s="2">
         <v>529</v>
       </c>
       <c r="D271" s="1" t="s">
@@ -12613,7 +13049,7 @@
       <c r="B272" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C272" s="1">
+      <c r="C272" s="2">
         <v>530</v>
       </c>
       <c r="D272" s="1" t="s">
@@ -12642,7 +13078,7 @@
       <c r="B273" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C273" s="1">
+      <c r="C273" s="2">
         <v>531</v>
       </c>
       <c r="D273" s="1" t="s">
@@ -12674,7 +13110,7 @@
       <c r="B274" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C274" s="1">
+      <c r="C274" s="2">
         <v>532</v>
       </c>
       <c r="D274" s="1" t="s">
@@ -12706,7 +13142,7 @@
       <c r="B275" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C275" s="1">
+      <c r="C275" s="2">
         <v>533</v>
       </c>
       <c r="D275" s="1" t="s">
@@ -12732,7 +13168,7 @@
       <c r="B276" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C276" s="1">
+      <c r="C276" s="2">
         <v>534</v>
       </c>
       <c r="D276" s="1" t="s">
@@ -12764,7 +13200,7 @@
       <c r="B277" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C277" s="1">
+      <c r="C277" s="2">
         <v>535</v>
       </c>
       <c r="D277" s="1" t="s">
@@ -12793,7 +13229,7 @@
       <c r="B278" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C278" s="1">
+      <c r="C278" s="2">
         <v>536</v>
       </c>
       <c r="D278" s="1" t="s">
@@ -12819,7 +13255,7 @@
       <c r="B279" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C279" s="1">
+      <c r="C279" s="2">
         <v>537</v>
       </c>
       <c r="D279" s="1" t="s">
@@ -12845,7 +13281,7 @@
       <c r="B280" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C280" s="1">
+      <c r="C280" s="2">
         <v>538</v>
       </c>
       <c r="D280" s="1" t="s">
@@ -12883,7 +13319,7 @@
       <c r="B281" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C281" s="1">
+      <c r="C281" s="2">
         <v>539</v>
       </c>
       <c r="D281" s="1" t="s">
@@ -12921,7 +13357,7 @@
       <c r="B282" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C282" s="1">
+      <c r="C282" s="2">
         <v>540</v>
       </c>
       <c r="D282" s="1" t="s">
@@ -12959,7 +13395,7 @@
       <c r="B283" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C283" s="1">
+      <c r="C283" s="2">
         <v>541</v>
       </c>
       <c r="D283" s="1" t="s">
@@ -12988,7 +13424,7 @@
       <c r="B284" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C284" s="1">
+      <c r="C284" s="2">
         <v>542</v>
       </c>
       <c r="D284" s="1" t="s">
@@ -13020,7 +13456,7 @@
       <c r="B285" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C285" s="1">
+      <c r="C285" s="2">
         <v>543</v>
       </c>
       <c r="D285" s="1" t="s">
@@ -13052,7 +13488,7 @@
       <c r="B286" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C286" s="1">
+      <c r="C286" s="2">
         <v>544</v>
       </c>
       <c r="D286" s="1" t="s">
@@ -13081,7 +13517,7 @@
       <c r="B287" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C287" s="1">
+      <c r="C287" s="2">
         <v>545</v>
       </c>
       <c r="D287" s="1" t="s">
@@ -13104,7 +13540,7 @@
       <c r="B288" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C288" s="1">
+      <c r="C288" s="2">
         <v>546</v>
       </c>
       <c r="D288" s="1" t="s">
@@ -13130,7 +13566,7 @@
       <c r="B289" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C289" s="1">
+      <c r="C289" s="2">
         <v>547</v>
       </c>
       <c r="D289" s="1" t="s">
@@ -13156,7 +13592,7 @@
       <c r="B290" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C290" s="1">
+      <c r="C290" s="2">
         <v>548</v>
       </c>
       <c r="D290" s="1" t="s">
@@ -13185,7 +13621,7 @@
       <c r="B291" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="C291" s="1">
+      <c r="C291" s="2">
         <v>549</v>
       </c>
       <c r="D291" s="1" t="s">
@@ -13212,6 +13648,1479 @@
       <c r="L291" s="1" t="s">
         <v>1329</v>
       </c>
+    </row>
+    <row r="292" spans="1:12" ht="54" x14ac:dyDescent="0.3">
+      <c r="A292" s="2">
+        <v>292</v>
+      </c>
+      <c r="B292" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>1331</v>
+      </c>
+      <c r="D292" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E292" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F292" s="3"/>
+      <c r="G292" s="3" t="s">
+        <v>1332</v>
+      </c>
+      <c r="H292" s="3"/>
+      <c r="I292" s="3"/>
+      <c r="J292" s="3"/>
+      <c r="K292" s="3"/>
+    </row>
+    <row r="293" spans="1:12" ht="36" x14ac:dyDescent="0.3">
+      <c r="A293" s="2">
+        <v>293</v>
+      </c>
+      <c r="B293" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C293" s="2">
+        <v>302</v>
+      </c>
+      <c r="D293" s="3" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E293" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F293" s="3"/>
+      <c r="G293" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="H293" s="3" t="s">
+        <v>1335</v>
+      </c>
+      <c r="I293" s="3"/>
+      <c r="J293" s="3"/>
+      <c r="K293" s="3"/>
+    </row>
+    <row r="294" spans="1:12" ht="54" x14ac:dyDescent="0.3">
+      <c r="A294" s="2">
+        <v>294</v>
+      </c>
+      <c r="B294" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C294" s="2">
+        <v>303</v>
+      </c>
+      <c r="D294" s="3" t="s">
+        <v>1336</v>
+      </c>
+      <c r="E294" s="3" t="s">
+        <v>1337</v>
+      </c>
+      <c r="F294" s="3" t="s">
+        <v>1338</v>
+      </c>
+      <c r="G294" s="3"/>
+      <c r="H294" s="3" t="s">
+        <v>1339</v>
+      </c>
+      <c r="I294" s="3" t="s">
+        <v>1340</v>
+      </c>
+      <c r="J294" s="3" t="s">
+        <v>1341</v>
+      </c>
+      <c r="K294" s="3"/>
+    </row>
+    <row r="295" spans="1:12" ht="54" x14ac:dyDescent="0.3">
+      <c r="A295" s="2">
+        <v>295</v>
+      </c>
+      <c r="B295" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C295" s="2">
+        <v>304</v>
+      </c>
+      <c r="D295" s="3" t="s">
+        <v>1342</v>
+      </c>
+      <c r="E295" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="F295" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G295" s="3"/>
+      <c r="H295" s="3" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I295" s="3" t="s">
+        <v>1344</v>
+      </c>
+      <c r="J295" s="3"/>
+      <c r="K295" s="3"/>
+    </row>
+    <row r="296" spans="1:12" ht="36" x14ac:dyDescent="0.3">
+      <c r="A296" s="2">
+        <v>296</v>
+      </c>
+      <c r="B296" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C296" s="2">
+        <v>305</v>
+      </c>
+      <c r="D296" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="E296" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F296" s="3"/>
+      <c r="G296" s="3"/>
+      <c r="H296" s="3" t="s">
+        <v>1345</v>
+      </c>
+      <c r="I296" s="3" t="s">
+        <v>1346</v>
+      </c>
+      <c r="J296" s="3"/>
+      <c r="K296" s="3"/>
+    </row>
+    <row r="297" spans="1:12" ht="36" x14ac:dyDescent="0.3">
+      <c r="A297" s="2">
+        <v>297</v>
+      </c>
+      <c r="B297" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C297" s="2">
+        <v>306</v>
+      </c>
+      <c r="D297" s="3" t="s">
+        <v>1347</v>
+      </c>
+      <c r="E297" s="3"/>
+      <c r="F297" s="3"/>
+      <c r="G297" s="3" t="s">
+        <v>1348</v>
+      </c>
+      <c r="H297" s="3" t="s">
+        <v>1349</v>
+      </c>
+      <c r="I297" s="3"/>
+      <c r="J297" s="3"/>
+      <c r="K297" s="3"/>
+    </row>
+    <row r="298" spans="1:12" ht="54" x14ac:dyDescent="0.3">
+      <c r="A298" s="2">
+        <v>298</v>
+      </c>
+      <c r="B298" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C298" s="2">
+        <v>307</v>
+      </c>
+      <c r="D298" s="3" t="s">
+        <v>1350</v>
+      </c>
+      <c r="E298" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F298" s="3"/>
+      <c r="G298" s="3" t="s">
+        <v>1351</v>
+      </c>
+      <c r="H298" s="3"/>
+      <c r="I298" s="3"/>
+      <c r="J298" s="3"/>
+      <c r="K298" s="3"/>
+    </row>
+    <row r="299" spans="1:12" ht="54" x14ac:dyDescent="0.3">
+      <c r="A299" s="2">
+        <v>299</v>
+      </c>
+      <c r="B299" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C299" s="2">
+        <v>308</v>
+      </c>
+      <c r="D299" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E299" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F299" s="3"/>
+      <c r="G299" s="3" t="s">
+        <v>1353</v>
+      </c>
+      <c r="H299" s="3" t="e">
+        <f>- wennsd Zeid hosd.</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="I299" s="3"/>
+      <c r="J299" s="3"/>
+      <c r="K299" s="3"/>
+    </row>
+    <row r="300" spans="1:12" ht="54" x14ac:dyDescent="0.3">
+      <c r="A300" s="2">
+        <v>300</v>
+      </c>
+      <c r="B300" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C300" s="2">
+        <v>309</v>
+      </c>
+      <c r="D300" s="3" t="s">
+        <v>1354</v>
+      </c>
+      <c r="E300" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F300" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="G300" s="3"/>
+      <c r="H300" s="3" t="s">
+        <v>1355</v>
+      </c>
+      <c r="I300" s="3" t="s">
+        <v>1356</v>
+      </c>
+      <c r="J300" s="3"/>
+      <c r="K300" s="3"/>
+    </row>
+    <row r="301" spans="1:12" ht="54" x14ac:dyDescent="0.3">
+      <c r="A301" s="2">
+        <v>301</v>
+      </c>
+      <c r="B301" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C301" s="2">
+        <v>310</v>
+      </c>
+      <c r="D301" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E301" s="3" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F301" s="3" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G301" s="3"/>
+      <c r="H301" s="3" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I301" s="3" t="e">
+        <f>-- und schlofn du ma a gern.</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="J301" s="3"/>
+      <c r="K301" s="3"/>
+    </row>
+    <row r="302" spans="1:12" ht="54" x14ac:dyDescent="0.3">
+      <c r="A302" s="2">
+        <v>302</v>
+      </c>
+      <c r="B302" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C302" s="2">
+        <v>311</v>
+      </c>
+      <c r="D302" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E302" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F302" s="3" t="s">
+        <v>1202</v>
+      </c>
+      <c r="G302" s="3"/>
+      <c r="H302" s="3" t="s">
+        <v>1360</v>
+      </c>
+      <c r="I302" s="3"/>
+      <c r="J302" s="3"/>
+      <c r="K302" s="3"/>
+    </row>
+    <row r="303" spans="1:12" ht="36" x14ac:dyDescent="0.3">
+      <c r="A303" s="2">
+        <v>303</v>
+      </c>
+      <c r="B303" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C303" s="2">
+        <v>312</v>
+      </c>
+      <c r="D303" s="3" t="s">
+        <v>1361</v>
+      </c>
+      <c r="E303" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F303" s="3"/>
+      <c r="G303" s="3" t="s">
+        <v>1362</v>
+      </c>
+      <c r="H303" s="3" t="s">
+        <v>1363</v>
+      </c>
+      <c r="I303" s="3"/>
+      <c r="J303" s="3"/>
+      <c r="K303" s="3"/>
+    </row>
+    <row r="304" spans="1:12" ht="36" x14ac:dyDescent="0.3">
+      <c r="A304" s="2">
+        <v>304</v>
+      </c>
+      <c r="B304" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C304" s="2">
+        <v>313</v>
+      </c>
+      <c r="D304" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E304" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F304" s="3" t="s">
+        <v>1364</v>
+      </c>
+      <c r="G304" s="3"/>
+      <c r="H304" s="3" t="s">
+        <v>1365</v>
+      </c>
+      <c r="I304" s="3"/>
+      <c r="J304" s="3"/>
+      <c r="K304" s="3"/>
+    </row>
+    <row r="305" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A305" s="2">
+        <v>305</v>
+      </c>
+      <c r="B305" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C305" s="2">
+        <v>314</v>
+      </c>
+      <c r="D305" s="3" t="s">
+        <v>1366</v>
+      </c>
+      <c r="E305" s="3" t="s">
+        <v>938</v>
+      </c>
+      <c r="F305" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="G305" s="3"/>
+      <c r="H305" s="3" t="s">
+        <v>1367</v>
+      </c>
+      <c r="I305" s="3"/>
+      <c r="J305" s="3"/>
+      <c r="K305" s="3"/>
+    </row>
+    <row r="306" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A306" s="2">
+        <v>306</v>
+      </c>
+      <c r="B306" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C306" s="2">
+        <v>315</v>
+      </c>
+      <c r="D306" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E306" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F306" s="3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G306" s="3"/>
+      <c r="H306" s="3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="I306" s="3" t="s">
+        <v>1370</v>
+      </c>
+      <c r="J306" s="3"/>
+      <c r="K306" s="3"/>
+    </row>
+    <row r="307" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A307" s="2">
+        <v>307</v>
+      </c>
+      <c r="B307" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C307" s="2">
+        <v>316</v>
+      </c>
+      <c r="D307" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E307" s="3" t="s">
+        <v>1371</v>
+      </c>
+      <c r="F307" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G307" s="3" t="s">
+        <v>1372</v>
+      </c>
+      <c r="H307" s="3"/>
+      <c r="I307" s="3" t="s">
+        <v>1373</v>
+      </c>
+      <c r="J307" s="3"/>
+      <c r="K307" s="3"/>
+    </row>
+    <row r="308" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A308" s="2">
+        <v>308</v>
+      </c>
+      <c r="B308" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C308" s="2">
+        <v>317</v>
+      </c>
+      <c r="D308" s="3" t="s">
+        <v>1374</v>
+      </c>
+      <c r="E308" s="3" t="s">
+        <v>1180</v>
+      </c>
+      <c r="F308" s="3"/>
+      <c r="G308" s="3" t="s">
+        <v>1375</v>
+      </c>
+      <c r="H308" s="3" t="s">
+        <v>1376</v>
+      </c>
+      <c r="I308" s="3"/>
+      <c r="J308" s="3"/>
+      <c r="K308" s="3"/>
+    </row>
+    <row r="309" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A309" s="2">
+        <v>309</v>
+      </c>
+      <c r="B309" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C309" s="2">
+        <v>318</v>
+      </c>
+      <c r="D309" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="E309" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F309" s="3"/>
+      <c r="G309" s="3" t="s">
+        <v>1377</v>
+      </c>
+      <c r="H309" s="3" t="s">
+        <v>1378</v>
+      </c>
+      <c r="I309" s="3"/>
+      <c r="J309" s="3"/>
+      <c r="K309" s="3"/>
+    </row>
+    <row r="310" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A310" s="2">
+        <v>310</v>
+      </c>
+      <c r="B310" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C310" s="2">
+        <v>319</v>
+      </c>
+      <c r="D310" s="3" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E310" s="3" t="s">
+        <v>1380</v>
+      </c>
+      <c r="F310" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G310" s="3"/>
+      <c r="H310" s="3" t="s">
+        <v>1381</v>
+      </c>
+      <c r="I310" s="3" t="s">
+        <v>1382</v>
+      </c>
+      <c r="J310" s="3"/>
+      <c r="K310" s="3"/>
+    </row>
+    <row r="311" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A311" s="2">
+        <v>311</v>
+      </c>
+      <c r="B311" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C311" s="2">
+        <v>320</v>
+      </c>
+      <c r="D311" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E311" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F311" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="G311" s="3"/>
+      <c r="H311" s="3" t="s">
+        <v>1384</v>
+      </c>
+      <c r="I311" s="3"/>
+      <c r="J311" s="3"/>
+      <c r="K311" s="3"/>
+    </row>
+    <row r="312" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A312" s="2">
+        <v>312</v>
+      </c>
+      <c r="B312" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C312" s="2">
+        <v>321</v>
+      </c>
+      <c r="D312" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E312" s="3" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F312" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="G312" s="3"/>
+      <c r="H312" s="3" t="s">
+        <v>1386</v>
+      </c>
+      <c r="I312" s="3"/>
+      <c r="J312" s="3"/>
+      <c r="K312" s="3"/>
+    </row>
+    <row r="313" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A313" s="2">
+        <v>313</v>
+      </c>
+      <c r="B313" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C313" s="2">
+        <v>322</v>
+      </c>
+      <c r="D313" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="E313" s="3" t="s">
+        <v>1338</v>
+      </c>
+      <c r="F313" s="3"/>
+      <c r="G313" s="3" t="s">
+        <v>1387</v>
+      </c>
+      <c r="H313" s="3" t="s">
+        <v>1388</v>
+      </c>
+      <c r="I313" s="3"/>
+      <c r="J313" s="3"/>
+      <c r="K313" s="3"/>
+    </row>
+    <row r="314" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A314" s="2">
+        <v>314</v>
+      </c>
+      <c r="B314" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C314" s="2">
+        <v>323</v>
+      </c>
+      <c r="D314" s="3" t="s">
+        <v>1389</v>
+      </c>
+      <c r="E314" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F314" s="3"/>
+      <c r="G314" s="3" t="s">
+        <v>1390</v>
+      </c>
+      <c r="H314" s="3" t="s">
+        <v>1391</v>
+      </c>
+      <c r="I314" s="3"/>
+      <c r="J314" s="3"/>
+      <c r="K314" s="3"/>
+    </row>
+    <row r="315" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A315" s="2">
+        <v>315</v>
+      </c>
+      <c r="B315" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C315" s="2">
+        <v>324</v>
+      </c>
+      <c r="D315" s="3" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E315" s="3" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F315" s="3"/>
+      <c r="G315" s="3" t="s">
+        <v>1394</v>
+      </c>
+      <c r="H315" s="3"/>
+      <c r="I315" s="3"/>
+      <c r="J315" s="3"/>
+      <c r="K315" s="3"/>
+    </row>
+    <row r="316" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A316" s="2">
+        <v>316</v>
+      </c>
+      <c r="B316" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C316" s="2">
+        <v>325</v>
+      </c>
+      <c r="D316" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E316" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F316" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G316" s="3"/>
+      <c r="H316" s="3" t="s">
+        <v>1395</v>
+      </c>
+      <c r="I316" s="3" t="s">
+        <v>1396</v>
+      </c>
+      <c r="J316" s="3" t="e">
+        <f>- sogn die Hexn baradox.</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K316" s="3"/>
+    </row>
+    <row r="317" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A317" s="2">
+        <v>317</v>
+      </c>
+      <c r="B317" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C317" s="2">
+        <v>326</v>
+      </c>
+      <c r="D317" s="3" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E317" s="3" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F317" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G317" s="3"/>
+      <c r="H317" s="3" t="s">
+        <v>1400</v>
+      </c>
+      <c r="I317" s="3" t="s">
+        <v>1401</v>
+      </c>
+      <c r="J317" s="3"/>
+      <c r="K317" s="3"/>
+    </row>
+    <row r="318" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A318" s="2">
+        <v>318</v>
+      </c>
+      <c r="B318" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C318" s="2">
+        <v>327</v>
+      </c>
+      <c r="D318" s="3" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E318" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F318" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G318" s="3"/>
+      <c r="H318" s="3" t="s">
+        <v>1403</v>
+      </c>
+      <c r="I318" s="3" t="e">
+        <f>- fia a Bridschn.</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="J318" s="3"/>
+      <c r="K318" s="3"/>
+    </row>
+    <row r="319" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A319" s="2">
+        <v>319</v>
+      </c>
+      <c r="B319" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C319" s="2">
+        <v>328</v>
+      </c>
+      <c r="D319" s="3" t="s">
+        <v>1404</v>
+      </c>
+      <c r="E319" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F319" s="3"/>
+      <c r="G319" s="3" t="s">
+        <v>1405</v>
+      </c>
+      <c r="H319" s="3" t="s">
+        <v>1406</v>
+      </c>
+      <c r="I319" s="3"/>
+      <c r="J319" s="3"/>
+      <c r="K319" s="3"/>
+    </row>
+    <row r="320" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A320" s="2">
+        <v>320</v>
+      </c>
+      <c r="B320" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C320" s="2">
+        <v>329</v>
+      </c>
+      <c r="D320" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="E320" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F320" s="3"/>
+      <c r="G320" s="3" t="s">
+        <v>1407</v>
+      </c>
+      <c r="H320" s="3" t="s">
+        <v>1408</v>
+      </c>
+      <c r="I320" s="3"/>
+      <c r="J320" s="3"/>
+      <c r="K320" s="3"/>
+    </row>
+    <row r="321" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A321" s="2">
+        <v>321</v>
+      </c>
+      <c r="B321" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C321" s="2">
+        <v>330</v>
+      </c>
+      <c r="D321" s="3" t="s">
+        <v>1409</v>
+      </c>
+      <c r="E321" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F321" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G321" s="3"/>
+      <c r="H321" s="3" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I321" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="J321" s="3" t="s">
+        <v>1412</v>
+      </c>
+      <c r="K321" s="3"/>
+    </row>
+    <row r="322" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A322" s="2">
+        <v>322</v>
+      </c>
+      <c r="B322" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C322" s="2">
+        <v>331</v>
+      </c>
+      <c r="D322" s="3" t="s">
+        <v>1413</v>
+      </c>
+      <c r="E322" s="3" t="s">
+        <v>1414</v>
+      </c>
+      <c r="F322" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="G322" s="3"/>
+      <c r="H322" s="3" t="s">
+        <v>1415</v>
+      </c>
+      <c r="I322" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="J322" s="3"/>
+      <c r="K322" s="3"/>
+    </row>
+    <row r="323" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A323" s="2">
+        <v>323</v>
+      </c>
+      <c r="B323" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C323" s="2">
+        <v>332</v>
+      </c>
+      <c r="D323" s="3" t="s">
+        <v>1417</v>
+      </c>
+      <c r="E323" s="3" t="s">
+        <v>1304</v>
+      </c>
+      <c r="F323" s="3"/>
+      <c r="G323" s="3" t="s">
+        <v>1418</v>
+      </c>
+      <c r="H323" s="3" t="s">
+        <v>1419</v>
+      </c>
+      <c r="I323" s="3"/>
+      <c r="J323" s="3"/>
+      <c r="K323" s="3"/>
+    </row>
+    <row r="324" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A324" s="2">
+        <v>324</v>
+      </c>
+      <c r="B324" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C324" s="2">
+        <v>333</v>
+      </c>
+      <c r="D324" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="E324" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="F324" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="G324" s="3"/>
+      <c r="H324" s="3" t="s">
+        <v>1420</v>
+      </c>
+      <c r="I324" s="3" t="s">
+        <v>1421</v>
+      </c>
+      <c r="J324" s="3"/>
+      <c r="K324" s="3"/>
+    </row>
+    <row r="325" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A325" s="2">
+        <v>325</v>
+      </c>
+      <c r="B325" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C325" s="2">
+        <v>334</v>
+      </c>
+      <c r="D325" s="3" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E325" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F325" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="G325" s="3"/>
+      <c r="H325" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="I325" s="3"/>
+      <c r="J325" s="3"/>
+      <c r="K325" s="3"/>
+    </row>
+    <row r="326" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A326" s="2">
+        <v>326</v>
+      </c>
+      <c r="B326" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C326" s="2">
+        <v>335</v>
+      </c>
+      <c r="D326" s="3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="E326" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="F326" s="3"/>
+      <c r="G326" s="3" t="s">
+        <v>1425</v>
+      </c>
+      <c r="H326" s="3" t="s">
+        <v>1426</v>
+      </c>
+      <c r="I326" s="3"/>
+      <c r="J326" s="3"/>
+      <c r="K326" s="3"/>
+    </row>
+    <row r="327" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A327" s="2">
+        <v>327</v>
+      </c>
+      <c r="B327" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C327" s="2">
+        <v>336</v>
+      </c>
+      <c r="D327" s="3" t="s">
+        <v>1427</v>
+      </c>
+      <c r="E327" s="3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="F327" s="3" t="s">
+        <v>1429</v>
+      </c>
+      <c r="G327" s="3"/>
+      <c r="H327" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="I327" s="3"/>
+      <c r="J327" s="3"/>
+      <c r="K327" s="3"/>
+    </row>
+    <row r="328" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A328" s="2">
+        <v>328</v>
+      </c>
+      <c r="B328" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C328" s="2">
+        <v>337</v>
+      </c>
+      <c r="D328" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E328" s="3" t="s">
+        <v>1431</v>
+      </c>
+      <c r="F328" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="G328" s="3"/>
+      <c r="H328" s="3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="I328" s="3" t="s">
+        <v>1433</v>
+      </c>
+      <c r="J328" s="3"/>
+      <c r="K328" s="3"/>
+    </row>
+    <row r="329" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A329" s="2">
+        <v>329</v>
+      </c>
+      <c r="B329" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C329" s="2">
+        <v>338</v>
+      </c>
+      <c r="D329" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="E329" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="F329" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="G329" s="3"/>
+      <c r="H329" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="I329" s="3" t="s">
+        <v>1435</v>
+      </c>
+      <c r="J329" s="3" t="s">
+        <v>1436</v>
+      </c>
+      <c r="K329" s="3"/>
+    </row>
+    <row r="330" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A330" s="2">
+        <v>330</v>
+      </c>
+      <c r="B330" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C330" s="2">
+        <v>339</v>
+      </c>
+      <c r="D330" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="E330" s="3" t="s">
+        <v>1438</v>
+      </c>
+      <c r="F330" s="3"/>
+      <c r="G330" s="3" t="s">
+        <v>1439</v>
+      </c>
+      <c r="H330" s="3"/>
+      <c r="I330" s="3"/>
+      <c r="J330" s="3"/>
+      <c r="K330" s="3"/>
+    </row>
+    <row r="331" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A331" s="2">
+        <v>331</v>
+      </c>
+      <c r="B331" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C331" s="2">
+        <v>340</v>
+      </c>
+      <c r="D331" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E331" s="3" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F331" s="3" t="s">
+        <v>1440</v>
+      </c>
+      <c r="G331" s="3" t="s">
+        <v>1441</v>
+      </c>
+      <c r="H331" s="3"/>
+      <c r="I331" s="3" t="s">
+        <v>1442</v>
+      </c>
+      <c r="J331" s="3" t="s">
+        <v>1443</v>
+      </c>
+      <c r="K331" s="3"/>
+    </row>
+    <row r="332" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A332" s="2">
+        <v>332</v>
+      </c>
+      <c r="B332" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C332" s="2">
+        <v>341</v>
+      </c>
+      <c r="D332" s="3" t="s">
+        <v>1444</v>
+      </c>
+      <c r="E332" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F332" s="3" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G332" s="3"/>
+      <c r="H332" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I332" s="3" t="s">
+        <v>1448</v>
+      </c>
+      <c r="J332" s="3"/>
+      <c r="K332" s="3"/>
+    </row>
+    <row r="333" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A333" s="2">
+        <v>333</v>
+      </c>
+      <c r="B333" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C333" s="2">
+        <v>342</v>
+      </c>
+      <c r="D333" s="3" t="s">
+        <v>1449</v>
+      </c>
+      <c r="E333" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F333" s="3"/>
+      <c r="G333" s="3" t="s">
+        <v>1450</v>
+      </c>
+      <c r="H333" s="3" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I333" s="3"/>
+      <c r="J333" s="3"/>
+      <c r="K333" s="3"/>
+    </row>
+    <row r="334" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A334" s="2">
+        <v>334</v>
+      </c>
+      <c r="B334" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C334" s="2">
+        <v>343</v>
+      </c>
+      <c r="D334" s="3" t="s">
+        <v>1452</v>
+      </c>
+      <c r="E334" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="F334" s="3" t="s">
+        <v>1453</v>
+      </c>
+      <c r="G334" s="3"/>
+      <c r="H334" s="3"/>
+      <c r="I334" s="3"/>
+      <c r="J334" s="3"/>
+      <c r="K334" s="3"/>
+    </row>
+    <row r="335" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A335" s="2">
+        <v>335</v>
+      </c>
+      <c r="B335" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C335" s="2">
+        <v>344</v>
+      </c>
+      <c r="D335" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="E335" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="F335" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G335" s="3"/>
+      <c r="H335" s="3" t="s">
+        <v>1454</v>
+      </c>
+      <c r="I335" s="3"/>
+      <c r="J335" s="3"/>
+      <c r="K335" s="3"/>
+    </row>
+    <row r="336" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A336" s="2">
+        <v>336</v>
+      </c>
+      <c r="B336" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C336" s="2">
+        <v>345</v>
+      </c>
+      <c r="D336" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E336" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F336" s="3" t="s">
+        <v>1455</v>
+      </c>
+      <c r="G336" s="3"/>
+      <c r="H336" s="3"/>
+      <c r="I336" s="3"/>
+      <c r="J336" s="3"/>
+      <c r="K336" s="3"/>
+    </row>
+    <row r="337" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A337" s="2">
+        <v>337</v>
+      </c>
+      <c r="B337" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C337" s="2">
+        <v>346</v>
+      </c>
+      <c r="D337" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E337" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="F337" s="3"/>
+      <c r="G337" s="3"/>
+      <c r="H337" s="3"/>
+      <c r="I337" s="3"/>
+      <c r="J337" s="3"/>
+      <c r="K337" s="3"/>
+    </row>
+    <row r="338" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A338" s="2">
+        <v>338</v>
+      </c>
+      <c r="B338" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C338" s="2">
+        <v>347</v>
+      </c>
+      <c r="D338" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E338" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F338" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="G338" s="3"/>
+      <c r="H338" s="3" t="s">
+        <v>1457</v>
+      </c>
+      <c r="I338" s="3" t="s">
+        <v>1458</v>
+      </c>
+      <c r="J338" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K338" s="3"/>
+    </row>
+    <row r="339" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A339" s="2">
+        <v>339</v>
+      </c>
+      <c r="B339" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C339" s="2">
+        <v>348</v>
+      </c>
+      <c r="D339" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E339" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F339" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="G339" s="3"/>
+      <c r="H339" s="3" t="s">
+        <v>1461</v>
+      </c>
+      <c r="I339" s="3" t="s">
+        <v>1462</v>
+      </c>
+      <c r="J339" s="3"/>
+      <c r="K339" s="3"/>
+    </row>
+    <row r="340" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A340" s="2">
+        <v>340</v>
+      </c>
+      <c r="B340" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C340" s="2">
+        <v>349</v>
+      </c>
+      <c r="D340" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E340" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="F340" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G340" s="3"/>
+      <c r="H340" s="3" t="s">
+        <v>1464</v>
+      </c>
+      <c r="I340" s="3" t="s">
+        <v>1465</v>
+      </c>
+      <c r="J340" s="3"/>
+      <c r="K340" s="3"/>
+    </row>
+    <row r="341" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A341" s="2">
+        <v>341</v>
+      </c>
+      <c r="B341" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C341" s="2">
+        <v>350</v>
+      </c>
+      <c r="D341" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="E341" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F341" s="3"/>
+      <c r="G341" s="3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="H341" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="I341" s="3"/>
+      <c r="J341" s="3"/>
+      <c r="K341" s="3"/>
+    </row>
+    <row r="342" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A342" s="2">
+        <v>342</v>
+      </c>
+      <c r="B342" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C342" s="2">
+        <v>351</v>
+      </c>
+      <c r="D342" s="3" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E342" s="3" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F342" s="3"/>
+      <c r="G342" s="3" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H342" s="3"/>
+      <c r="I342" s="3"/>
+      <c r="J342" s="3"/>
+      <c r="K342" s="3"/>
+    </row>
+    <row r="343" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A343" s="2">
+        <v>343</v>
+      </c>
+      <c r="B343" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C343" s="2">
+        <v>352</v>
+      </c>
+      <c r="D343" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="E343" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="F343" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G343" s="3"/>
+      <c r="H343" s="3" t="s">
+        <v>1469</v>
+      </c>
+      <c r="I343" s="3" t="s">
+        <v>1470</v>
+      </c>
+      <c r="J343" s="3"/>
+      <c r="K343" s="3"/>
+    </row>
+    <row r="344" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+      <c r="A344" s="2">
+        <v>344</v>
+      </c>
+      <c r="B344" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C344" s="2">
+        <v>353</v>
+      </c>
+      <c r="D344" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E344" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F344" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G344" s="3"/>
+      <c r="H344" s="3" t="s">
+        <v>1471</v>
+      </c>
+      <c r="I344" s="3" t="s">
+        <v>1472</v>
+      </c>
+      <c r="J344" s="3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="K344" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>